<commit_message>
Added queries for agg_sales and fix dim_model png
Signed-off-by: Cátia Teixeira <catia.rds.teixeira@gmail.com>
</commit_message>
<xml_diff>
--- a/Model-designs/Dictionaries_v2.xlsx
+++ b/Model-designs/Dictionaries_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmigu\Downloads\DW_project-main (2)\DW_project-main\Model-designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\FEUP\MDSE\Data Warehousing\Project\Model-designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7C9D42-7EB2-43AF-A18D-C7D037049242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AA85BD-BB54-4DEC-A786-2A176932C1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{107B6A6F-3B59-46BE-8B41-F06765D6C700}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{107B6A6F-3B59-46BE-8B41-F06765D6C700}"/>
   </bookViews>
   <sheets>
     <sheet name="Facts" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="170">
   <si>
     <t>Name</t>
   </si>
@@ -544,10 +544,10 @@
     <t>sales, order_item_total</t>
   </si>
   <si>
-    <t>sales_per_customer, weekly_sales, monthly_sales</t>
-  </si>
-  <si>
     <t>1 / month / week</t>
+  </si>
+  <si>
+    <t>sales_per_segment, weekly_sales, monthly_sales</t>
   </si>
 </sst>
 </file>
@@ -923,7 +923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -957,6 +957,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -972,10 +975,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -994,7 +993,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1292,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7CB58F-A90E-494D-87A4-EF24C5DA7232}">
   <dimension ref="B2:Q22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1356,24 +1355,24 @@
       <c r="Q4" s="24"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="K5" s="27" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
+      <c r="K5" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="25" t="s">
@@ -1555,15 +1554,15 @@
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
       <c r="H13" s="24"/>
-      <c r="K13" s="27" t="s">
+      <c r="K13" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="26" t="s">
@@ -1653,15 +1652,15 @@
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="26" t="s">
@@ -1717,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A7CB72-7E08-4F61-8D4C-0C558E9858F5}">
   <dimension ref="B2:AR16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13:P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO24" sqref="AO24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2374,7 +2373,7 @@
       </c>
       <c r="AR10" s="12"/>
     </row>
-    <row r="11" spans="2:44" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
         <v>14</v>
       </c>
@@ -2424,21 +2423,21 @@
         <v>32</v>
       </c>
       <c r="Z11" s="12"/>
-      <c r="AC11" s="11" t="s">
+      <c r="AC11" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AD11" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1" t="s">
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AH11" s="1">
+      <c r="AH11" s="14">
         <v>4</v>
       </c>
-      <c r="AI11" s="12"/>
+      <c r="AI11" s="15"/>
       <c r="AL11" s="11" t="s">
         <v>112</v>
       </c>
@@ -2552,7 +2551,7 @@
       <c r="O13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P13" s="33">
+      <c r="P13" s="1">
         <v>15</v>
       </c>
       <c r="Q13" s="12"/>
@@ -2622,7 +2621,7 @@
       <c r="O14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P14" s="33">
+      <c r="P14" s="1">
         <v>15</v>
       </c>
       <c r="Q14" s="12"/>
@@ -2661,7 +2660,7 @@
       </c>
       <c r="AR14" s="12"/>
     </row>
-    <row r="15" spans="2:44" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
@@ -2696,42 +2695,42 @@
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="12"/>
-      <c r="T15" s="1" t="s">
+      <c r="T15" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="U15" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="V15" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="W15" s="1" t="s">
+      <c r="W15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="X15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y15" s="1">
-        <v>32</v>
-      </c>
-      <c r="Z15" s="12"/>
-      <c r="AL15" s="11" t="s">
+      <c r="X15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y15" s="14">
+        <v>32</v>
+      </c>
+      <c r="Z15" s="15"/>
+      <c r="AL15" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="AM15" s="1"/>
-      <c r="AN15" s="11" t="s">
+      <c r="AM15" s="14"/>
+      <c r="AN15" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="AO15" s="1" t="s">
+      <c r="AO15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AP15" s="1" t="s">
+      <c r="AP15" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AQ15" s="1">
+      <c r="AQ15" s="14">
         <v>4</v>
       </c>
-      <c r="AR15" s="12"/>
+      <c r="AR15" s="15"/>
     </row>
     <row r="16" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="13" t="s">
@@ -2749,29 +2748,29 @@
       <c r="F16" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="14">
         <v>32</v>
       </c>
       <c r="H16" s="15"/>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="M16" s="14" t="s">
         <v>90</v>
       </c>
       <c r="N16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P16" s="1">
+      <c r="O16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P16" s="14">
         <v>320</v>
       </c>
-      <c r="Q16" s="12"/>
+      <c r="Q16" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2783,7 +2782,7 @@
   <dimension ref="B3:H7"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2795,12 +2794,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="2:8" ht="116.4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -2829,7 +2828,7 @@
       <c r="B5" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="27" t="s">
         <v>165</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -2869,11 +2868,11 @@
       <c r="B7" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>168</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>169</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>83</v>
@@ -2884,9 +2883,7 @@
       <c r="G7" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>83</v>
-      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>